<commit_message>
Preparing new evaluations to run.
#windowsbytecodes
</commit_message>
<xml_diff>
--- a/results/2017-03-18 - avgDelayTest/Stats.xlsx
+++ b/results/2017-03-18 - avgDelayTest/Stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -307,16 +307,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>430</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>291</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>311</c:v>
+                  <c:v>336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>322</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,16 +389,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>582</c:v>
+                  <c:v>584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>865</c:v>
+                  <c:v>852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>730</c:v>
+                  <c:v>716</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>744</c:v>
+                  <c:v>587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -413,11 +413,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="376785520"/>
-        <c:axId val="376787480"/>
+        <c:axId val="300364528"/>
+        <c:axId val="300361784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="376785520"/>
+        <c:axId val="300364528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,12 +474,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376787480"/>
+        <c:crossAx val="300361784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376787480"/>
+        <c:axId val="300361784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +536,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376785520"/>
+        <c:crossAx val="300364528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1561,7 @@
         <v>19</v>
       </c>
       <c r="L2">
-        <v>430</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>22</v>
       </c>
       <c r="L3">
-        <v>291</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
         <v>25</v>
       </c>
       <c r="L4">
-        <v>311</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>28</v>
       </c>
       <c r="L5">
-        <v>322</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>32</v>
       </c>
       <c r="L6">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>35</v>
       </c>
       <c r="L7">
-        <v>865</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1789,7 +1789,7 @@
         <v>38</v>
       </c>
       <c r="L8">
-        <v>730</v>
+        <v>716</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1827,7 +1827,7 @@
         <v>41</v>
       </c>
       <c r="L9">
-        <v>744</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>